<commit_message>
hotel categories scores added
</commit_message>
<xml_diff>
--- a/data_structure.xlsx
+++ b/data_structure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gerardalcaldegascon/Library/CloudStorage/OneDrive-UniversitatObertadeCatalunya/2. Master Data Science/Semestre 3/Tipologia y ciclo de vida de los datos/PRA 1/WebScrapingUOC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C8D4554D-963E-B34F-A8F8-EEA666BD9603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC79ECB3-9A75-AD4D-9CD4-15A48C5B5D06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{3EA3FD3A-924C-CE47-BBBC-201ADE7EAA75}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17500" xr2:uid="{3EA3FD3A-924C-CE47-BBBC-201ADE7EAA75}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>Estructura de los datos a almacenar</t>
   </si>
@@ -44,9 +44,6 @@
     <t>name</t>
   </si>
   <si>
-    <t>direction</t>
-  </si>
-  <si>
     <t>[Vistas a la ciudad, Admite mascotas, …]</t>
   </si>
   <si>
@@ -62,9 +59,6 @@
     <t>list</t>
   </si>
   <si>
-    <t>description</t>
-  </si>
-  <si>
     <t>popular_services</t>
   </si>
   <si>
@@ -108,6 +102,30 @@
   </si>
   <si>
     <t>Será un diccionario si puedo extraer el nombre de cada categoria</t>
+  </si>
+  <si>
+    <t>hotel_score</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>8.5</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>hotel_description</t>
+  </si>
+  <si>
+    <t>list of strings</t>
+  </si>
+  <si>
+    <t>hotel_scores</t>
+  </si>
+  <si>
+    <t>key for category</t>
   </si>
 </sst>
 </file>
@@ -462,144 +480,162 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B80490A-CF6B-894E-B9FB-88871ADC1017}">
-  <dimension ref="C4:L12"/>
+  <dimension ref="C4:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="13.6640625" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" customWidth="1"/>
-    <col min="5" max="5" width="35" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" customWidth="1"/>
-    <col min="8" max="8" width="16.83203125" customWidth="1"/>
-    <col min="11" max="11" width="25.5" customWidth="1"/>
+    <col min="4" max="6" width="17.6640625" customWidth="1"/>
+    <col min="7" max="7" width="35" customWidth="1"/>
+    <col min="8" max="9" width="15.33203125" customWidth="1"/>
+    <col min="10" max="10" width="16.83203125" customWidth="1"/>
+    <col min="13" max="13" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
     </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" t="s">
         <v>6</v>
       </c>
-      <c r="D7" t="s">
+      <c r="H7" t="s">
         <v>6</v>
       </c>
-      <c r="E7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
+      <c r="I7" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
     </row>
-    <row r="8" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="H8" t="s">
+    <row r="8" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="I8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" t="s">
+        <v>10</v>
+      </c>
+      <c r="K8" t="s">
+        <v>11</v>
+      </c>
+      <c r="L8" t="s">
         <v>12</v>
       </c>
-      <c r="I8" t="s">
+      <c r="M8" t="s">
         <v>13</v>
       </c>
-      <c r="J8" t="s">
+      <c r="N8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="J9" t="s">
+        <v>5</v>
+      </c>
+      <c r="K9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L9" t="s">
+        <v>15</v>
+      </c>
+      <c r="M9" t="s">
+        <v>6</v>
+      </c>
+      <c r="N9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" t="s">
+        <v>2</v>
+      </c>
+      <c r="J10" t="s">
         <v>14</v>
       </c>
-      <c r="K8" t="s">
-        <v>15</v>
-      </c>
-      <c r="L8" t="s">
+      <c r="K10">
+        <v>2</v>
+      </c>
+      <c r="L10">
+        <v>285</v>
+      </c>
+      <c r="M10" t="s">
+        <v>16</v>
+      </c>
+      <c r="N10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="H9" t="s">
-        <v>6</v>
-      </c>
-      <c r="I9" t="s">
-        <v>17</v>
-      </c>
-      <c r="J9" t="s">
-        <v>17</v>
-      </c>
-      <c r="K9" t="s">
-        <v>7</v>
-      </c>
-      <c r="L9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>4</v>
-      </c>
-      <c r="E10" t="s">
-        <v>3</v>
-      </c>
-      <c r="H10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10">
-        <v>2</v>
-      </c>
-      <c r="J10">
-        <v>285</v>
-      </c>
-      <c r="K10" t="s">
-        <v>18</v>
-      </c>
-      <c r="L10" t="s">
+    <row r="12" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="N12" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="L12" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="H7:L7"/>
-    <mergeCell ref="H6:L6"/>
+    <mergeCell ref="J7:N7"/>
+    <mergeCell ref="J6:N6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>